<commit_message>
Limpeza: removidos arquivos temporários e pastas ignoradas pelo .gitignore
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -40,10 +40,29 @@
     <t xml:space="preserve">Ana</t>
   </si>
   <si>
-    <t xml:space="preserve">Olá, sou o robo do gustavo!</t>
+    <t xml:space="preserve">(61)98182-6392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/gustavo/Downloads/95743d639b4ea4d15c740d7a973c548f.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">dhiogenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guilherme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá Professor(a), tudo bem?
+Aqui quem fala é Matheus Xavier da NT Editora.
+Tomo a liberdade de encaminhar essa mensagem no intuito de compartilhar o nosso Catálogo de Livros e Catálogo descritivo da nossa Biblioteca Virtual para a Formação Técnica e Profissional.
+Sabemos do desafio que é o fornecimento de materiais didáticos de qualidade e com foco no aluno do ensino profissional. Face ao exposto, gostaria de agendar uma rápida apresentação das nossas soluções educacionais que irão contribuir com a oferta da Vossa Instituição de Ensino.
+Podemos falar?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thiago </t>
   </si>
 </sst>
 </file>
@@ -54,7 +73,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -75,6 +94,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -119,7 +143,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -130,6 +154,14 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -149,16 +181,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="57.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -182,22 +215,47 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>5561981826392</v>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5561982757272</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>6</v>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>61984850276</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>61994187913</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Melhorias no script e add PDF no disparador
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -37,16 +37,19 @@
     <t xml:space="preserve">Imagem</t>
   </si>
   <si>
+    <t xml:space="preserve">PDF</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ana</t>
   </si>
   <si>
     <t xml:space="preserve">(61)98182-6392</t>
   </si>
   <si>
-    <t xml:space="preserve">ola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/gustavo/Downloads/95743d639b4ea4d15c740d7a973c548f.jpg</t>
+    <t xml:space="preserve">imagens/galo.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDF/BV NT - Catálogo.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">dhiogenes</t>
@@ -160,7 +163,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -181,17 +184,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="57.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.06"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -210,52 +214,56 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5561982757272</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>61984850276</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>61994187913</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Melhorias no disparo.py e interface; suporte a envio de imagem e PDF separados
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -40,22 +40,10 @@
     <t xml:space="preserve">PDF</t>
   </si>
   <si>
-    <t xml:space="preserve">Ana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(61)98182-6392</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imagens/galo.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDF/BV NT - Catálogo.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dhiogenes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">guilherme</t>
+    <t xml:space="preserve">teste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(61)98446-8993</t>
   </si>
   <si>
     <t xml:space="preserve">Olá Professor(a), tudo bem?
@@ -65,7 +53,7 @@
 Podemos falar?</t>
   </si>
   <si>
-    <t xml:space="preserve">thiago </t>
+    <t xml:space="preserve">/home/gustavo/Desktop/meus_projetos/whatsapp_disparador/PDF/catalogo.pdf</t>
   </si>
 </sst>
 </file>
@@ -146,7 +134,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -159,11 +147,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -184,18 +168,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="57.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="66.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="66.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -218,52 +202,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>5561982757272</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>61984850276</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>61994187913</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>